<commit_message>
v0.5.6 - Artemis orgs, devices, crew
</commit_message>
<xml_diff>
--- a/output/CodeSystem-aerospace-behavioral-state-cs.xlsx
+++ b/output/CodeSystem-aerospace-behavioral-state-cs.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.5.5</t>
+    <t>0.5.6</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-30T10:45:53-07:00</t>
+    <t>2025-12-30T13:15:27-07:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>